<commit_message>
added python script for connecting to a twitter feed
</commit_message>
<xml_diff>
--- a/Evaluation of Classification Models/Supplemental Material/Calculating Weighted Confusion Matrix.xlsx
+++ b/Evaluation of Classification Models/Supplemental Material/Calculating Weighted Confusion Matrix.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10092" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Threshold Optimization Using We" sheetId="1" r:id="rId1"/>
@@ -584,12 +584,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1253,7 +1254,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{758374A1-F9F0-46F2-A228-11A0BD50FCA8}" type="CELLRANGE">
+                    <a:fld id="{ECCBF9B9-8DAB-42EB-BB40-DB6C0A6ED462}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1286,7 +1287,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{162D3B8F-79E3-4AF4-8ACD-CDCC49421C3F}" type="CELLRANGE">
+                    <a:fld id="{A1EF7251-5B83-4662-9B28-191EB803F1E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1319,7 +1320,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E278773-9117-4D4E-AC2A-CDD71C2BB99E}" type="CELLRANGE">
+                    <a:fld id="{AF88EB21-8461-4095-86D7-5B763C1BBBF6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1352,7 +1353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32A312E6-D85D-4235-8105-2BC8B5EB9D39}" type="CELLRANGE">
+                    <a:fld id="{8CF08699-81FE-4A6C-B85F-16E7BD9388C9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1385,7 +1386,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D65EE513-CFAF-46F1-8DAC-308323082071}" type="CELLRANGE">
+                    <a:fld id="{ECBE58C5-3B93-4943-8A9D-3D03046B69D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1418,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F339C26C-13D8-4825-A53D-1DABA934F271}" type="CELLRANGE">
+                    <a:fld id="{1F2867A8-B13F-458E-9705-FA4327B2233C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1451,7 +1452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9B1D2FC8-CF9E-4BB3-8EE9-A42CB70157D5}" type="CELLRANGE">
+                    <a:fld id="{8B65F335-597C-4635-8F23-962B2B9E9AD7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1485,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21158F84-C18F-4AF8-AB1D-A3625E534EB9}" type="CELLRANGE">
+                    <a:fld id="{48BFC77C-A753-415F-B5F8-193EF55D9B5B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1517,7 +1518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C3D1C14-C211-4663-BDE3-17370DA23116}" type="CELLRANGE">
+                    <a:fld id="{D3DDB19D-FC8C-404A-BF49-62814DBF3138}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1550,7 +1551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DFEF257-845B-4B25-B7F0-3C61B7D2460F}" type="CELLRANGE">
+                    <a:fld id="{81A32EE3-AE37-4C76-93EC-493F2939E25D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1583,7 +1584,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B0BC1A7-463C-450B-A057-0096473934D4}" type="CELLRANGE">
+                    <a:fld id="{310AC0CC-F87E-4214-8EA6-28CF24088625}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1758,37 +1759,37 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="11"/>
                   <c:pt idx="0">
-                    <c:v>0</c:v>
+                    <c:v>0.00%</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1</c:v>
+                    <c:v>10.00%</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.2</c:v>
+                    <c:v>20.00%</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.3</c:v>
+                    <c:v>30.00%</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4</c:v>
+                    <c:v>40.00%</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.5</c:v>
+                    <c:v>50.00%</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.6</c:v>
+                    <c:v>60.00%</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.7</c:v>
+                    <c:v>70.00%</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.8</c:v>
+                    <c:v>80.00%</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0.9</c:v>
+                    <c:v>90.00%</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>1</c:v>
+                    <c:v>100.00%</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2071,7 +2072,7 @@
             <c:numRef>
               <c:f>'Roc Calculations'!$A$2:$A$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2174,7 +2175,7 @@
             <c:numRef>
               <c:f>'Roc Calculations'!$A$2:$A$12</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2294,7 +2295,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4685,8 +4686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N274"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="F7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12359,13 +12360,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
@@ -12376,7 +12377,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B1" t="s">
@@ -12411,7 +12412,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2">
@@ -12440,7 +12441,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>0.1</v>
       </c>
       <c r="B3">
@@ -12481,7 +12482,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>0.2</v>
       </c>
       <c r="B4">
@@ -12510,7 +12511,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>0.3</v>
       </c>
       <c r="B5">
@@ -12546,7 +12547,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>0.4</v>
       </c>
       <c r="B6">
@@ -12582,7 +12583,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>0.5</v>
       </c>
       <c r="B7">
@@ -12618,7 +12619,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>0.6</v>
       </c>
       <c r="B8">
@@ -12654,7 +12655,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>0.7</v>
       </c>
       <c r="B9">
@@ -12690,7 +12691,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>0.8</v>
       </c>
       <c r="B10">
@@ -12726,7 +12727,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>0.9</v>
       </c>
       <c r="B11">
@@ -12755,7 +12756,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12">
@@ -12785,6 +12786,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>